<commit_message>
Add new notebook and update edgecases
</commit_message>
<xml_diff>
--- a/Data/Edgecases.xlsx
+++ b/Data/Edgecases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Malcolm/Documents/GitHub/Fantasyland/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Malcolm/Documents/GitHub/Fantasyland/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EDB89A5-8858-3143-A90E-C9941FFBF918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10DF9F2-0EB8-F94A-8C25-AC6B53345EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{DF2B0E2F-E263-AF44-9DF2-4F2A0CA96ABD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -52,12 +52,6 @@
     <t>[('8', 'Spades'), ('9', 'Diamonds'), ('10', 'Clubs'), ('J', 'Hearts'), ('Q', 'Hearts'), ('Q', 'Clubs'), ('Q', 'Diamonds'), ('10', 'Hearts'), ('A', 'Spades'), ('2', 'Clubs'), ('2', 'Hearts'), ('3', 'Diamonds'), ('5', 'Clubs')]</t>
   </si>
   <si>
-    <t>Contains 3 Queens where the the Queen of Diamonds is part of a 5 card flush</t>
-  </si>
-  <si>
-    <t>Contains 3 Queens where the Queen rank is part of a 8,9,10,J,Q (Q-high) straight.</t>
-  </si>
-  <si>
     <t>[('10', 'Diamonds'), ('2', 'Clubs'),('3', 'Hearts'),('4', 'Diamonds'),('5', 'Hearts'),('6', 'Hearts'),('8', 'Spades'),('9', 'Diamonds'),('A', 'Clubs'),('A', 'Hearts'),('J', 'Spades'),('A', 'Diamonds'),('Q', 'Diamonds')]</t>
   </si>
   <si>
@@ -65,9 +59,6 @@
   </si>
   <si>
     <t>One card from each rank</t>
-  </si>
-  <si>
-    <t>A pair and 2,3,4,5,6 and 8,9,10,J,Q straights</t>
   </si>
   <si>
     <t>01_threequeens_edgecase_flush_str</t>
@@ -98,10 +89,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">[('4', 'Diamonds'), ('5', 'Hearts'), ('5', 'Diamonds'), ('6', 'Spades'), ('7', 'Spades'), ('7', 'Hearts'), ('7', 'Clubs'), ('7', 'Diamonds'), ('8', 'Spades'), ('8', 'Diamonds'), ('9', 'Hearts'), ('10', 'Diamonds'), ('J', 'Diamonds'),]
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">[('4', 'Diamonds'), ('5', 'Hearts'), ('5', 'Diamonds'), ('6', 'Spades'), ('6', 'Diamonds'), ('7', 'Spades'), ('7', 'Hearts'), ('7', 'Clubs'), ('7', 'Diamonds'), ('8', 'Spades'), ('9', 'Hearts'), ('10', 'Diamonds'), ('J', 'Diamonds'),]
 </t>
   </si>
@@ -112,15 +99,6 @@
     <t>08_interaction_flush_got_2_straight_1_good_straight</t>
   </si>
   <si>
-    <t>Contains a 2 straight, and a flush</t>
-  </si>
-  <si>
-    <t xml:space="preserve">('9', 'Diamonds') is subed for ('9', 'Hearts'). Thereby, making the 9-high straight the only viable one </t>
-  </si>
-  <si>
-    <t>('8', 'Diamonds') is subed for ('6', 'Diamonds'). 2 straights no longer found because central cards 7 and 8 are not duplicate.</t>
-  </si>
-  <si>
     <t>10_2_long_straight_involving_ACES</t>
   </si>
   <si>
@@ -140,6 +118,37 @@
   </si>
   <si>
     <t>[('2', 'Hearts', 'ID_12'), ('3', 'Spades', 'ID_8'), ('3', 'Diamonds', 'ID_4'), ('4', 'Spades', 'ID_7'), ('5', 'Diamonds', 'ID_11'), ('7', 'Spades', 'ID_1'), ('8', 'Diamonds', 'ID_6'), ('9', 'Spades', 'ID_10'), ('10', 'Diamonds', 'ID_3'), ('J', 'Diamonds', 'ID_9'), ('Q', 'Spades', 'ID_2'), ('K', 'Diamonds', 'ID_13'), ('A', 'Diamonds', 'ID_5')]</t>
+  </si>
+  <si>
+    <t>Contains 3 Queens where the the Queen of Diamonds is part of a 5 card flush. No fantasy</t>
+  </si>
+  <si>
+    <t>Contains 3 Queens where the Queen rank is part of a 8,9,10,J,Q (Q-high) straight.No Fantasy</t>
+  </si>
+  <si>
+    <t>A pair and 2,3,4,5,6 and 8,9,10,J,Q straights.Fantasy</t>
+  </si>
+  <si>
+    <t>triggers fantast for double kings, and quad 10, perhaps develop for all 13 synergy?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[('4', 'Diamonds'), ('5', 'Hearts'), ('5', 'Diamonds'), ('6', 'Spades'), ('7', 'Spades'), ('7', 'Hearts'), ('7', 'Clubs'), ('7', 'Diamonds'), ('8', 'Spades'), ('8', 'Diamonds'), ('9', 'Hearts'), ('10', 'Diamonds'), ('J', 'Diamonds')]
+</t>
+  </si>
+  <si>
+    <t>Contains a 2 straight, and a flush. Classic Case_1 Both Flush and One Long straight from 4 to J inclusive bounds.</t>
+  </si>
+  <si>
+    <t>('9', 'Diamonds') is subed for ('9', 'Hearts'). This time there are no loaned_flushed_cards</t>
+  </si>
+  <si>
+    <t>A couple of 5's, Ace-Low, and Ace-High straights. No Fantasy.</t>
+  </si>
+  <si>
+    <t>Continueing from prev TC, ('8', 'Diamonds') is subed for ('6', 'Diamonds'). 2 straights no longer found because central cards 7 and 8 are not duplicate. This actually doesn't factor because it is case_1, expected result bad TC.</t>
+  </si>
+  <si>
+    <t>Hardcoded 3 monsters, namely quad 10s, diamond flush and 9-A straight.</t>
   </si>
 </sst>
 </file>
@@ -497,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF0DCDF-CA70-BE49-A1E2-B9B130C8C33E}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,119 +530,128 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhanced Case2 problem by limiting straights
</commit_message>
<xml_diff>
--- a/Data/Edgecases.xlsx
+++ b/Data/Edgecases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Malcolm/Documents/GitHub/Fantasyland/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10DF9F2-0EB8-F94A-8C25-AC6B53345EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB49A8AC-60BC-354D-B776-556DCB5E9E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{DF2B0E2F-E263-AF44-9DF2-4F2A0CA96ABD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -149,6 +149,15 @@
   </si>
   <si>
     <t>Hardcoded 3 monsters, namely quad 10s, diamond flush and 9-A straight.</t>
+  </si>
+  <si>
+    <t>13_Case2_</t>
+  </si>
+  <si>
+    <t>[('A', 'Spades'), ('A', 'Hearts'), ('A', 'Clubs'), ('2', 'Spades'), ('4', 'Hearts'), ('5', 'Clubs'), ('6', 'Diamonds'), ('7', 'Spades'), ('8', 'Hearts'), ('9', 'Clubs'), ('9', 'Diamonds'), ('10','Clubs'), ('10', 'Diamonds')]</t>
+  </si>
+  <si>
+    <t>Needed to improve test_dim function with tuple, so each straight in Case 2 is registered properly.</t>
   </si>
 </sst>
 </file>
@@ -504,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF0DCDF-CA70-BE49-A1E2-B9B130C8C33E}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -654,6 +663,17 @@
         <v>26</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>